<commit_message>
changed emergence check method - check last ten steps for emergence
</commit_message>
<xml_diff>
--- a/outputs/b_emergence_check.xlsx
+++ b/outputs/b_emergence_check.xlsx
@@ -557,10 +557,10 @@
         <v>0.1</v>
       </c>
       <c r="N2" t="n">
-        <v>56.79012345679012</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>43.20987654320987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -610,10 +610,10 @@
         <v>0.1</v>
       </c>
       <c r="N3" t="n">
-        <v>37.03703703703704</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>62.96296296296296</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -663,10 +663,10 @@
         <v>0.15</v>
       </c>
       <c r="N4" t="n">
-        <v>51.85185185185185</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>48.14814814814815</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -716,10 +716,10 @@
         <v>0.05</v>
       </c>
       <c r="N5" t="n">
-        <v>53.125</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>46.875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -769,10 +769,10 @@
         <v>0.15</v>
       </c>
       <c r="N6" t="n">
-        <v>42.1875</v>
+        <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>57.8125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -822,10 +822,10 @@
         <v>0.15</v>
       </c>
       <c r="N7" t="n">
-        <v>59.375</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>40.625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -875,10 +875,10 @@
         <v>0.05</v>
       </c>
       <c r="N8" t="n">
-        <v>49.38271604938272</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>50.61728395061728</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -928,10 +928,10 @@
         <v>0.1</v>
       </c>
       <c r="N9" t="n">
-        <v>51.85185185185185</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>48.14814814814815</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -981,10 +981,10 @@
         <v>0.2</v>
       </c>
       <c r="N10" t="n">
-        <v>49.38271604938272</v>
+        <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>50.61728395061728</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1034,10 +1034,10 @@
         <v>0.1</v>
       </c>
       <c r="N11" t="n">
-        <v>53.125</v>
+        <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>46.875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1087,10 +1087,10 @@
         <v>0.15</v>
       </c>
       <c r="N12" t="n">
-        <v>51.5625</v>
+        <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>48.4375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1140,10 +1140,10 @@
         <v>0.15</v>
       </c>
       <c r="N13" t="n">
-        <v>35.9375</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>64.0625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1193,10 +1193,10 @@
         <v>0.2</v>
       </c>
       <c r="N14" t="n">
-        <v>46.875</v>
+        <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>53.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1246,10 +1246,10 @@
         <v>0.2</v>
       </c>
       <c r="N15" t="n">
-        <v>54.6875</v>
+        <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>45.3125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1299,10 +1299,10 @@
         <v>0.2</v>
       </c>
       <c r="N16" t="n">
-        <v>43.20987654320987</v>
+        <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>56.79012345679012</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1352,10 +1352,10 @@
         <v>0.2</v>
       </c>
       <c r="N17" t="n">
-        <v>51.85185185185185</v>
+        <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>48.14814814814815</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1405,10 +1405,10 @@
         <v>0.1</v>
       </c>
       <c r="N18" t="n">
-        <v>62.96296296296296</v>
+        <v>0</v>
       </c>
       <c r="O18" t="n">
-        <v>37.03703703703704</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1458,10 +1458,10 @@
         <v>0.2</v>
       </c>
       <c r="N19" t="n">
-        <v>41.9753086419753</v>
+        <v>0</v>
       </c>
       <c r="O19" t="n">
-        <v>58.0246913580247</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1511,10 +1511,10 @@
         <v>0.05</v>
       </c>
       <c r="N20" t="n">
-        <v>46.875</v>
+        <v>0</v>
       </c>
       <c r="O20" t="n">
-        <v>53.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1564,10 +1564,10 @@
         <v>0.15</v>
       </c>
       <c r="N21" t="n">
-        <v>53.125</v>
+        <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>46.875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1617,10 +1617,10 @@
         <v>0.2</v>
       </c>
       <c r="N22" t="n">
-        <v>45.3125</v>
+        <v>0</v>
       </c>
       <c r="O22" t="n">
-        <v>54.6875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1670,10 +1670,10 @@
         <v>0.05</v>
       </c>
       <c r="N23" t="n">
-        <v>46.875</v>
+        <v>0</v>
       </c>
       <c r="O23" t="n">
-        <v>53.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1723,10 +1723,10 @@
         <v>0.05</v>
       </c>
       <c r="N24" t="n">
-        <v>46.875</v>
+        <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>53.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1776,10 +1776,10 @@
         <v>0.05</v>
       </c>
       <c r="N25" t="n">
-        <v>45.3125</v>
+        <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>54.6875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1829,10 +1829,10 @@
         <v>0.1</v>
       </c>
       <c r="N26" t="n">
-        <v>48.4375</v>
+        <v>0</v>
       </c>
       <c r="O26" t="n">
-        <v>51.5625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1882,10 +1882,10 @@
         <v>0.1</v>
       </c>
       <c r="N27" t="n">
-        <v>54.6875</v>
+        <v>0</v>
       </c>
       <c r="O27" t="n">
-        <v>45.3125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1935,10 +1935,10 @@
         <v>0.1</v>
       </c>
       <c r="N28" t="n">
-        <v>46.875</v>
+        <v>0</v>
       </c>
       <c r="O28" t="n">
-        <v>53.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1988,10 +1988,10 @@
         <v>0.15</v>
       </c>
       <c r="N29" t="n">
-        <v>54.6875</v>
+        <v>0</v>
       </c>
       <c r="O29" t="n">
-        <v>45.3125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -2041,10 +2041,10 @@
         <v>0.05</v>
       </c>
       <c r="N30" t="n">
-        <v>58.0246913580247</v>
+        <v>0</v>
       </c>
       <c r="O30" t="n">
-        <v>41.9753086419753</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -2094,10 +2094,10 @@
         <v>0.05</v>
       </c>
       <c r="N31" t="n">
-        <v>48.14814814814815</v>
+        <v>0</v>
       </c>
       <c r="O31" t="n">
-        <v>51.85185185185185</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -2147,10 +2147,10 @@
         <v>0.05</v>
       </c>
       <c r="N32" t="n">
-        <v>49.38271604938272</v>
+        <v>0</v>
       </c>
       <c r="O32" t="n">
-        <v>50.61728395061728</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -2200,10 +2200,10 @@
         <v>0.05</v>
       </c>
       <c r="N33" t="n">
-        <v>39.50617283950617</v>
+        <v>0</v>
       </c>
       <c r="O33" t="n">
-        <v>60.49382716049383</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -2253,10 +2253,10 @@
         <v>0.1</v>
       </c>
       <c r="N34" t="n">
-        <v>40.74074074074074</v>
+        <v>0</v>
       </c>
       <c r="O34" t="n">
-        <v>59.25925925925925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -2306,10 +2306,10 @@
         <v>0.1</v>
       </c>
       <c r="N35" t="n">
-        <v>46.91358024691358</v>
+        <v>0</v>
       </c>
       <c r="O35" t="n">
-        <v>53.08641975308642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -2359,10 +2359,10 @@
         <v>0.15</v>
       </c>
       <c r="N36" t="n">
-        <v>55.55555555555556</v>
+        <v>0</v>
       </c>
       <c r="O36" t="n">
-        <v>44.44444444444444</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -2412,10 +2412,10 @@
         <v>0.15</v>
       </c>
       <c r="N37" t="n">
-        <v>39.50617283950617</v>
+        <v>0</v>
       </c>
       <c r="O37" t="n">
-        <v>60.49382716049383</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -2465,10 +2465,10 @@
         <v>0.2</v>
       </c>
       <c r="N38" t="n">
-        <v>50.61728395061728</v>
+        <v>0</v>
       </c>
       <c r="O38" t="n">
-        <v>49.38271604938272</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -2518,7 +2518,7 @@
         <v>0.2</v>
       </c>
       <c r="N39" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O39" t="n">
         <v>0</v>
@@ -2571,7 +2571,7 @@
         <v>0.2</v>
       </c>
       <c r="N40" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="O40" t="n">
         <v>0</v>
@@ -2624,10 +2624,10 @@
         <v>0.1</v>
       </c>
       <c r="N41" t="n">
-        <v>45.3125</v>
+        <v>0</v>
       </c>
       <c r="O41" t="n">
-        <v>54.6875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -2677,10 +2677,10 @@
         <v>0.15</v>
       </c>
       <c r="N42" t="n">
-        <v>45.3125</v>
+        <v>0</v>
       </c>
       <c r="O42" t="n">
-        <v>54.6875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -2730,10 +2730,10 @@
         <v>0.05</v>
       </c>
       <c r="N43" t="n">
-        <v>53.08641975308642</v>
+        <v>0</v>
       </c>
       <c r="O43" t="n">
-        <v>46.91358024691358</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -2783,10 +2783,10 @@
         <v>0.05</v>
       </c>
       <c r="N44" t="n">
-        <v>56.79012345679012</v>
+        <v>0</v>
       </c>
       <c r="O44" t="n">
-        <v>43.20987654320987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -2836,10 +2836,10 @@
         <v>0.05</v>
       </c>
       <c r="N45" t="n">
-        <v>46.91358024691358</v>
+        <v>0</v>
       </c>
       <c r="O45" t="n">
-        <v>53.08641975308642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -2889,10 +2889,10 @@
         <v>0.1</v>
       </c>
       <c r="N46" t="n">
-        <v>46.91358024691358</v>
+        <v>0</v>
       </c>
       <c r="O46" t="n">
-        <v>53.08641975308642</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -2942,10 +2942,10 @@
         <v>0.15</v>
       </c>
       <c r="N47" t="n">
-        <v>45.67901234567901</v>
+        <v>0</v>
       </c>
       <c r="O47" t="n">
-        <v>54.32098765432099</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -2995,10 +2995,10 @@
         <v>0.15</v>
       </c>
       <c r="N48" t="n">
-        <v>61.72839506172839</v>
+        <v>0</v>
       </c>
       <c r="O48" t="n">
-        <v>38.2716049382716</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -3048,10 +3048,10 @@
         <v>0.2</v>
       </c>
       <c r="N49" t="n">
-        <v>48.14814814814815</v>
+        <v>0</v>
       </c>
       <c r="O49" t="n">
-        <v>51.85185185185185</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -3101,10 +3101,10 @@
         <v>0.2</v>
       </c>
       <c r="N50" t="n">
-        <v>40.74074074074074</v>
+        <v>0</v>
       </c>
       <c r="O50" t="n">
-        <v>59.25925925925925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -3154,10 +3154,10 @@
         <v>0.2</v>
       </c>
       <c r="N51" t="n">
-        <v>49.38271604938272</v>
+        <v>0</v>
       </c>
       <c r="O51" t="n">
-        <v>50.61728395061728</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -3207,10 +3207,10 @@
         <v>0.2</v>
       </c>
       <c r="N52" t="n">
-        <v>51.85185185185185</v>
+        <v>0</v>
       </c>
       <c r="O52" t="n">
-        <v>48.14814814814815</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>